<commit_message>
Documentos Finales para visto bueno
Guion pasado a formato .doc para dejar ecuaciones como imágenes, mapa
conceptual y recursos revisados.

Cordial saludo.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion02/CN_10_02_CO.xlsx
+++ b/fuentes/contenidos/grado10/guion02/CN_10_02_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="11760" tabRatio="729"/>
+    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="11760" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -28,61 +28,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>MARIANELA CUELLAR</author>
-  </authors>
-  <commentList>
-    <comment ref="E24" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Preguntar por imagen
-y por la ficha del alumno que también tiene imagen, se hace necesario formato</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E44" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Preguntar sobre foto dentro de tabla</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E47" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Preguntar sobre foto dentro de tabla</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="72">
   <si>
     <t>FICHA</t>
   </si>
@@ -178,9 +125,6 @@
   </si>
   <si>
     <t>Identifica las unidades de las magnitudes físicas cinemáticas</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: EL movimiento</t>
   </si>
   <si>
     <t>Movimiento rectilíneo uniforme</t>
@@ -307,7 +251,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -373,13 +317,6 @@
       <family val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Cambria"/>
@@ -422,7 +359,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -439,12 +376,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
         <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -924,7 +855,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -963,55 +894,52 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="401">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1694,7 +1622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1725,7 +1653,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1768,7 +1696,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1809,16 +1737,16 @@
         <v>10</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F2" s="18">
         <v>1</v>
@@ -1835,16 +1763,16 @@
         <v>10</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F3" s="18">
         <v>3</v>
@@ -1855,22 +1783,22 @@
         <v>10</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F4" s="19">
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1878,16 +1806,16 @@
         <v>10</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F5" s="19">
         <v>6</v>
@@ -1898,16 +1826,16 @@
         <v>10</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F6" s="19">
         <v>8</v>
@@ -1918,22 +1846,22 @@
         <v>10</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" s="23" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F7" s="23">
         <v>9</v>
       </c>
       <c r="G7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1941,22 +1869,22 @@
         <v>10</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" s="23" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F8" s="23">
         <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1964,16 +1892,16 @@
         <v>10</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="23" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F9" s="23">
         <v>11</v>
@@ -1985,16 +1913,16 @@
         <v>10</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="37" t="s">
-        <v>67</v>
+      <c r="D10" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="36" t="s">
+        <v>66</v>
       </c>
       <c r="F10" s="26">
         <v>14</v>
@@ -2006,22 +1934,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" s="26" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="37" t="s">
-        <v>67</v>
+        <v>49</v>
+      </c>
+      <c r="E11" s="36" t="s">
+        <v>66</v>
       </c>
       <c r="F11" s="26">
         <v>15</v>
       </c>
       <c r="G11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -2029,16 +1957,16 @@
         <v>10</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C12" s="26" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>67</v>
+        <v>50</v>
+      </c>
+      <c r="E12" s="36" t="s">
+        <v>66</v>
       </c>
       <c r="F12" s="26">
         <v>16</v>
@@ -2050,68 +1978,68 @@
         <v>10</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="37" t="s">
-        <v>67</v>
+      <c r="D13" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="36" t="s">
+        <v>66</v>
       </c>
       <c r="F13" s="26">
         <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="39">
+      <c r="A14" s="38">
         <v>10</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="38" t="s">
         <v>66</v>
-      </c>
-      <c r="C14" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="39" t="s">
-        <v>67</v>
       </c>
       <c r="F14" s="30">
         <v>19</v>
       </c>
       <c r="G14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="39">
+      <c r="A15" s="38">
         <v>10</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="38" t="s">
         <v>66</v>
-      </c>
-      <c r="C15" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="39" t="s">
-        <v>67</v>
       </c>
       <c r="F15" s="30">
         <v>20</v>
       </c>
       <c r="G15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2163,7 +2091,7 @@
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>30</v>
@@ -2173,8 +2101,8 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
-        <v>38</v>
+      <c r="A4" s="35" t="s">
+        <v>37</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>30</v>
@@ -2185,7 +2113,7 @@
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="23" t="s">
         <v>30</v>
@@ -2196,7 +2124,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>30</v>
@@ -2206,10 +2134,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="37" t="s">
+      <c r="A7" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="36" t="s">
         <v>30</v>
       </c>
       <c r="C7" s="26">
@@ -2218,7 +2146,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="33" t="s">
         <v>30</v>
@@ -2229,7 +2157,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="33" t="s">
         <v>30</v>
@@ -2260,7 +2188,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2286,10 +2214,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>59</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2297,7 +2225,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>30</v>
@@ -2308,10 +2236,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2319,7 +2247,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>30</v>
@@ -2330,10 +2258,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2341,18 +2269,18 @@
         <v>6</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>7</v>
       </c>
-      <c r="B8" s="36" t="s">
-        <v>62</v>
+      <c r="B8" s="35" t="s">
+        <v>61</v>
       </c>
       <c r="C8" s="19" t="s">
         <v>30</v>
@@ -2363,10 +2291,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2374,10 +2302,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2385,10 +2313,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2396,10 +2324,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2407,7 +2335,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" s="23" t="s">
         <v>30</v>
@@ -2418,7 +2346,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="23" t="s">
         <v>30</v>
@@ -2428,11 +2356,11 @@
       <c r="A15" s="26">
         <v>14</v>
       </c>
-      <c r="B15" s="37" t="s">
-        <v>48</v>
+      <c r="B15" s="36" t="s">
+        <v>47</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2440,10 +2368,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2451,29 +2379,29 @@
         <v>16</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="26">
         <v>17</v>
       </c>
-      <c r="B18" s="38" t="s">
-        <v>52</v>
+      <c r="B18" s="37" t="s">
+        <v>51</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="26">
         <v>18</v>
       </c>
-      <c r="B19" s="37" t="s">
-        <v>53</v>
+      <c r="B19" s="36" t="s">
+        <v>52</v>
       </c>
       <c r="C19" s="26" t="s">
         <v>30</v>
@@ -2483,22 +2411,22 @@
       <c r="A20" s="30">
         <v>19</v>
       </c>
-      <c r="B20" s="39" t="s">
-        <v>55</v>
+      <c r="B20" s="38" t="s">
+        <v>54</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="30">
         <v>20</v>
       </c>
-      <c r="B21" s="39" t="s">
-        <v>56</v>
+      <c r="B21" s="38" t="s">
+        <v>55</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2506,7 +2434,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" s="33" t="s">
         <v>30</v>
@@ -2517,7 +2445,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C23" s="33" t="s">
         <v>30</v>
@@ -2542,12 +2470,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I78"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView topLeftCell="D3" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2562,19 +2488,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="39" t="s">
         <v>17</v>
       </c>
       <c r="F1" s="17" t="s">
@@ -2583,16 +2509,16 @@
       <c r="G1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="40" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>23</v>
@@ -2609,7 +2535,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>23</v>
@@ -2626,7 +2552,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>23</v>
@@ -2643,7 +2569,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>23</v>
@@ -2660,14 +2586,14 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E6" s="20" t="s">
         <v>24</v>
@@ -2679,14 +2605,14 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>25</v>
@@ -2698,14 +2624,14 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>24</v>
@@ -2717,14 +2643,14 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>27</v>
@@ -2736,14 +2662,14 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>24</v>
@@ -2755,14 +2681,14 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>25</v>
@@ -2774,14 +2700,14 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>24</v>
@@ -2793,14 +2719,14 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>25</v>
@@ -2812,14 +2738,14 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E14" s="20" t="s">
         <v>25</v>
@@ -2831,14 +2757,14 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E15" s="20" t="s">
         <v>24</v>
@@ -2850,14 +2776,14 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>28</v>
@@ -2865,15 +2791,15 @@
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
       <c r="H16" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" s="18" t="s">
         <v>59</v>
-      </c>
-      <c r="I16" s="18" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>23</v>
@@ -2892,7 +2818,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>23</v>
@@ -2907,7 +2833,7 @@
       <c r="F18" s="20"/>
       <c r="G18" s="20"/>
       <c r="H18" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I18" s="18" t="s">
         <v>30</v>
@@ -2915,7 +2841,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>23</v>
@@ -2930,18 +2856,18 @@
       <c r="F19" s="20"/>
       <c r="G19" s="20"/>
       <c r="H19" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I19" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="19" t="s">
         <v>24</v>
@@ -2955,10 +2881,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="19" t="s">
         <v>26</v>
@@ -2972,10 +2898,10 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" s="19" t="s">
         <v>28</v>
@@ -2985,7 +2911,7 @@
       <c r="F22" s="21"/>
       <c r="G22" s="21"/>
       <c r="H22" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I22" s="19" t="s">
         <v>30</v>
@@ -2993,16 +2919,16 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" s="19"/>
       <c r="D23" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="19" t="s">
         <v>24</v>
       </c>
       <c r="F23" s="21"/>
@@ -3012,16 +2938,16 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" s="19"/>
       <c r="D24" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="E24" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="19" t="s">
         <v>25</v>
       </c>
       <c r="F24" s="21"/>
@@ -3031,16 +2957,16 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" s="19"/>
       <c r="D25" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="E25" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="19" t="s">
         <v>25</v>
       </c>
       <c r="F25" s="21"/>
@@ -3050,14 +2976,14 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26" s="19"/>
       <c r="D26" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E26" s="21" t="s">
         <v>24</v>
@@ -3069,14 +2995,14 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E27" s="21" t="s">
         <v>25</v>
@@ -3088,14 +3014,14 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C28" s="19"/>
       <c r="D28" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E28" s="21" t="s">
         <v>24</v>
@@ -3107,37 +3033,37 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" s="19"/>
       <c r="D29" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="21" t="s">
         <v>35</v>
-      </c>
-      <c r="E29" s="21" t="s">
-        <v>36</v>
       </c>
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
       <c r="H29" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I29" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30" s="19"/>
       <c r="D30" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E30" s="21" t="s">
         <v>28</v>
@@ -3145,18 +3071,18 @@
       <c r="F30" s="21"/>
       <c r="G30" s="21"/>
       <c r="H30" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I30" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="21" t="s">
@@ -3172,10 +3098,10 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32" s="19"/>
       <c r="D32" s="21" t="s">
@@ -3186,8 +3112,8 @@
       </c>
       <c r="F32" s="21"/>
       <c r="G32" s="21"/>
-      <c r="H32" s="36" t="s">
-        <v>62</v>
+      <c r="H32" s="35" t="s">
+        <v>61</v>
       </c>
       <c r="I32" s="19" t="s">
         <v>30</v>
@@ -3195,10 +3121,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C33" s="19"/>
       <c r="D33" s="21" t="s">
@@ -3210,18 +3136,18 @@
       <c r="F33" s="21"/>
       <c r="G33" s="21"/>
       <c r="H33" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I33" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C34" s="23" t="s">
         <v>24</v>
@@ -3235,10 +3161,10 @@
     </row>
     <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C35" s="23" t="s">
         <v>26</v>
@@ -3252,10 +3178,10 @@
     </row>
     <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C36" s="23" t="s">
         <v>24</v>
@@ -3269,10 +3195,10 @@
     </row>
     <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C37" s="23" t="s">
         <v>25</v>
@@ -3286,10 +3212,10 @@
     </row>
     <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B38" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C38" s="23" t="s">
         <v>24</v>
@@ -3303,10 +3229,10 @@
     </row>
     <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C39" s="23" t="s">
         <v>27</v>
@@ -3320,10 +3246,10 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C40" s="23" t="s">
         <v>28</v>
@@ -3333,18 +3259,18 @@
       <c r="F40" s="25"/>
       <c r="G40" s="25"/>
       <c r="H40" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I40" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B41" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C41" s="23" t="s">
         <v>24</v>
@@ -3358,10 +3284,10 @@
     </row>
     <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C42" s="23" t="s">
         <v>27</v>
@@ -3375,14 +3301,14 @@
     </row>
     <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B43" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C43" s="23"/>
       <c r="D43" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E43" s="25" t="s">
         <v>24</v>
@@ -3394,16 +3320,16 @@
     </row>
     <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B44" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C44" s="23"/>
       <c r="D44" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="E44" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44" s="23" t="s">
         <v>25</v>
       </c>
       <c r="F44" s="25"/>
@@ -3413,16 +3339,16 @@
     </row>
     <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C45" s="23"/>
       <c r="D45" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="E45" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="E45" s="23" t="s">
         <v>25</v>
       </c>
       <c r="F45" s="25"/>
@@ -3432,16 +3358,16 @@
     </row>
     <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C46" s="23"/>
       <c r="D46" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="E46" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E46" s="23" t="s">
         <v>24</v>
       </c>
       <c r="F46" s="25"/>
@@ -3451,16 +3377,16 @@
     </row>
     <row r="47" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B47" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C47" s="23"/>
       <c r="D47" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="E47" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="E47" s="23" t="s">
         <v>25</v>
       </c>
       <c r="F47" s="25"/>
@@ -3470,16 +3396,16 @@
     </row>
     <row r="48" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B48" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C48" s="23"/>
       <c r="D48" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="E48" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="E48" s="23" t="s">
         <v>25</v>
       </c>
       <c r="F48" s="25"/>
@@ -3489,14 +3415,14 @@
     </row>
     <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B49" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C49" s="23"/>
       <c r="D49" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E49" s="25" t="s">
         <v>25</v>
@@ -3508,14 +3434,14 @@
     </row>
     <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B50" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C50" s="23"/>
       <c r="D50" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E50" s="25" t="s">
         <v>25</v>
@@ -3527,37 +3453,37 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C51" s="23"/>
       <c r="D51" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E51" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F51" s="25"/>
       <c r="G51" s="25"/>
       <c r="H51" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I51" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C52" s="23"/>
       <c r="D52" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E52" s="25" t="s">
         <v>28</v>
@@ -3565,18 +3491,18 @@
       <c r="F52" s="25"/>
       <c r="G52" s="25"/>
       <c r="H52" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I52" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B53" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C53" s="23"/>
       <c r="D53" s="25" t="s">
@@ -3592,10 +3518,10 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C54" s="23"/>
       <c r="D54" s="25" t="s">
@@ -3607,7 +3533,7 @@
       <c r="F54" s="25"/>
       <c r="G54" s="25"/>
       <c r="H54" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I54" s="23" t="s">
         <v>30</v>
@@ -3615,10 +3541,10 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C55" s="23"/>
       <c r="D55" s="25" t="s">
@@ -3630,7 +3556,7 @@
       <c r="F55" s="25"/>
       <c r="G55" s="25"/>
       <c r="H55" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I55" s="23" t="s">
         <v>30</v>
@@ -3638,10 +3564,10 @@
     </row>
     <row r="56" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B56" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C56" s="26" t="s">
         <v>24</v>
@@ -3655,10 +3581,10 @@
     </row>
     <row r="57" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B57" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C57" s="26" t="s">
         <v>26</v>
@@ -3672,10 +3598,10 @@
     </row>
     <row r="58" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B58" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C58" s="26" t="s">
         <v>25</v>
@@ -3689,10 +3615,10 @@
     </row>
     <row r="59" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B59" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C59" s="26" t="s">
         <v>24</v>
@@ -3706,10 +3632,10 @@
     </row>
     <row r="60" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B60" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C60" s="26" t="s">
         <v>25</v>
@@ -3723,10 +3649,10 @@
     </row>
     <row r="61" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B61" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C61" s="26" t="s">
         <v>24</v>
@@ -3740,10 +3666,10 @@
     </row>
     <row r="62" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B62" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C62" s="26" t="s">
         <v>25</v>
@@ -3757,10 +3683,10 @@
     </row>
     <row r="63" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B63" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C63" s="26" t="s">
         <v>24</v>
@@ -3774,35 +3700,35 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B64" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C64" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D64" s="28"/>
       <c r="E64" s="28"/>
       <c r="F64" s="28"/>
       <c r="G64" s="28"/>
-      <c r="H64" s="37" t="s">
-        <v>48</v>
+      <c r="H64" s="36" t="s">
+        <v>47</v>
       </c>
       <c r="I64" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C65" s="26"/>
       <c r="D65" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E65" s="28" t="s">
         <v>24</v>
@@ -3814,14 +3740,14 @@
     </row>
     <row r="66" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B66" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C66" s="26"/>
       <c r="D66" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E66" s="28" t="s">
         <v>25</v>
@@ -3833,14 +3759,14 @@
     </row>
     <row r="67" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B67" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C67" s="26"/>
       <c r="D67" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E67" s="28" t="s">
         <v>26</v>
@@ -3852,37 +3778,37 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B68" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C68" s="26"/>
-      <c r="D68" s="42" t="s">
-        <v>49</v>
+      <c r="D68" s="41" t="s">
+        <v>48</v>
       </c>
       <c r="E68" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F68" s="28"/>
       <c r="G68" s="28"/>
       <c r="H68" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I68" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B69" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C69" s="26"/>
-      <c r="D69" s="42" t="s">
-        <v>49</v>
+      <c r="D69" s="41" t="s">
+        <v>48</v>
       </c>
       <c r="E69" s="28" t="s">
         <v>28</v>
@@ -3890,41 +3816,41 @@
       <c r="F69" s="28"/>
       <c r="G69" s="28"/>
       <c r="H69" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I69" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B70" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C70" s="26"/>
-      <c r="D70" s="42" t="s">
-        <v>49</v>
+      <c r="D70" s="41" t="s">
+        <v>48</v>
       </c>
       <c r="E70" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F70" s="28"/>
       <c r="G70" s="28"/>
-      <c r="H70" s="38" t="s">
-        <v>52</v>
+      <c r="H70" s="37" t="s">
+        <v>51</v>
       </c>
       <c r="I70" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B71" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C71" s="26"/>
       <c r="D71" s="28" t="s">
@@ -3940,10 +3866,10 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B72" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C72" s="26"/>
       <c r="D72" s="28" t="s">
@@ -3954,8 +3880,8 @@
       </c>
       <c r="F72" s="28"/>
       <c r="G72" s="28"/>
-      <c r="H72" s="37" t="s">
-        <v>53</v>
+      <c r="H72" s="36" t="s">
+        <v>52</v>
       </c>
       <c r="I72" s="26" t="s">
         <v>30</v>
@@ -3963,10 +3889,10 @@
     </row>
     <row r="73" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B73" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C73" s="30" t="s">
         <v>24</v>
@@ -3980,10 +3906,10 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B74" s="30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C74" s="30" t="s">
         <v>28</v>
@@ -3992,19 +3918,19 @@
       <c r="E74" s="32"/>
       <c r="F74" s="32"/>
       <c r="G74" s="32"/>
-      <c r="H74" s="39" t="s">
-        <v>55</v>
+      <c r="H74" s="38" t="s">
+        <v>54</v>
       </c>
       <c r="I74" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B75" s="30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C75" s="30" t="s">
         <v>28</v>
@@ -4013,19 +3939,19 @@
       <c r="E75" s="32"/>
       <c r="F75" s="32"/>
       <c r="G75" s="32"/>
-      <c r="H75" s="39" t="s">
-        <v>56</v>
+      <c r="H75" s="38" t="s">
+        <v>55</v>
       </c>
       <c r="I75" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B76" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C76" s="33"/>
       <c r="D76" s="34"/>
@@ -4039,10 +3965,10 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B77" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C77" s="33"/>
       <c r="D77" s="34"/>
@@ -4050,22 +3976,15 @@
       <c r="F77" s="34"/>
       <c r="G77" s="34"/>
       <c r="H77" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I77" s="33" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I78" s="5">
-        <f>COUNTA(I2:I77)</f>
-        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>